<commit_message>
Moved column id_parametro from table etapas to table fases_etapas, so that each action can have its own setpoint if needed.
</commit_message>
<xml_diff>
--- a/MySQL/configuration/etapas.xlsx
+++ b/MySQL/configuration/etapas.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\UNIOVI\Master\IntegracionDeSistemas\TrabajoIntegracion\DockerIntegracion\MySQL\configuration\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB69A6DE-B179-4E2F-B655-F501564CF781}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{746B9E6F-3AE3-4ED3-AB98-434858B1FD5D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>id_etapa</t>
   </si>
@@ -33,9 +33,6 @@
     <t>id_receta_maestra</t>
   </si>
   <si>
-    <t>id_parametro</t>
-  </si>
-  <si>
     <t>nombre</t>
   </si>
   <si>
@@ -52,9 +49,6 @@
   </si>
   <si>
     <t>E2</t>
-  </si>
-  <si>
-    <t>NULL</t>
   </si>
 </sst>
 </file>
@@ -372,10 +366,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H8" sqref="H8"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -385,7 +379,7 @@
     <col min="3" max="3" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -401,31 +395,25 @@
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
+      <c r="D2">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>1</v>
-      </c>
-      <c r="C2" t="s">
-        <v>9</v>
-      </c>
-      <c r="D2" t="s">
-        <v>6</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -433,19 +421,16 @@
         <v>1</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
-      </c>
-      <c r="D3" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
       </c>
       <c r="E3">
         <v>0</v>
       </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -453,15 +438,12 @@
         <v>1</v>
       </c>
       <c r="C4" t="s">
-        <v>9</v>
-      </c>
-      <c r="D4" t="s">
-        <v>8</v>
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
       </c>
       <c r="E4">
-        <v>0</v>
-      </c>
-      <c r="F4">
         <v>1</v>
       </c>
     </row>

</xml_diff>